<commit_message>
Example of dB mapping. However, with rounding errors (because of int and not float).
</commit_message>
<xml_diff>
--- a/Documentation/DB_Mapping.xlsx
+++ b/Documentation/DB_Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oddbj\Documents\git\Revelator.io24.Api\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E02CB45-7B57-4646-9ED2-5448FDBA4838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4957118-5490-469E-9FD6-BC6DE699BCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{4EF7F543-1A19-4AA0-AC06-25240FBC5CDA}"/>
+    <workbookView xWindow="-21720" yWindow="-9810" windowWidth="21840" windowHeight="38040" xr2:uid="{4EF7F543-1A19-4AA0-AC06-25240FBC5CDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Volume Mic L" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -107,13 +108,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1956,7 +1958,7 @@
   <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC17" sqref="AC17"/>
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,8 +1996,8 @@
       <c r="B3" s="2">
         <v>0.97350000000000003</v>
       </c>
-      <c r="C3" s="3">
-        <f>B2-B3</f>
+      <c r="C3" s="6">
+        <f t="shared" ref="C3:C32" si="0">B2-B3</f>
         <v>2.6499999999999968E-2</v>
       </c>
     </row>
@@ -2006,8 +2008,8 @@
       <c r="B4" s="2">
         <v>0.94699997000000002</v>
       </c>
-      <c r="C4" s="3">
-        <f>B3-B4</f>
+      <c r="C4" s="6">
+        <f t="shared" si="0"/>
         <v>2.6500030000000008E-2</v>
       </c>
     </row>
@@ -2018,8 +2020,8 @@
       <c r="B5" s="2">
         <v>0.92049999999999998</v>
       </c>
-      <c r="C5" s="3">
-        <f>B4-B5</f>
+      <c r="C5" s="6">
+        <f t="shared" si="0"/>
         <v>2.6499970000000039E-2</v>
       </c>
     </row>
@@ -2030,8 +2032,8 @@
       <c r="B6" s="2">
         <v>0.89400000000000002</v>
       </c>
-      <c r="C6" s="3">
-        <f>B5-B6</f>
+      <c r="C6" s="6">
+        <f t="shared" si="0"/>
         <v>2.6499999999999968E-2</v>
       </c>
     </row>
@@ -2042,8 +2044,8 @@
       <c r="B7" s="2">
         <v>0.86749995000000002</v>
       </c>
-      <c r="C7" s="3">
-        <f>B6-B7</f>
+      <c r="C7" s="6">
+        <f t="shared" si="0"/>
         <v>2.6500049999999997E-2</v>
       </c>
     </row>
@@ -2054,8 +2056,8 @@
       <c r="B8" s="2">
         <v>0.84099995999999999</v>
       </c>
-      <c r="C8" s="3">
-        <f>B7-B8</f>
+      <c r="C8" s="6">
+        <f t="shared" si="0"/>
         <v>2.6499990000000029E-2</v>
       </c>
     </row>
@@ -2066,8 +2068,8 @@
       <c r="B9" s="2">
         <v>0.8145</v>
       </c>
-      <c r="C9" s="3">
-        <f>B8-B9</f>
+      <c r="C9" s="6">
+        <f t="shared" si="0"/>
         <v>2.6499959999999989E-2</v>
       </c>
     </row>
@@ -2078,8 +2080,8 @@
       <c r="B10" s="2">
         <v>0.78800000000000003</v>
       </c>
-      <c r="C10" s="3">
-        <f>B9-B10</f>
+      <c r="C10" s="6">
+        <f t="shared" si="0"/>
         <v>2.6499999999999968E-2</v>
       </c>
     </row>
@@ -2090,8 +2092,8 @@
       <c r="B11" s="2">
         <v>0.76149999999999995</v>
       </c>
-      <c r="C11" s="3">
-        <f>B10-B11</f>
+      <c r="C11" s="6">
+        <f t="shared" si="0"/>
         <v>2.6500000000000079E-2</v>
       </c>
     </row>
@@ -2102,8 +2104,8 @@
       <c r="B12" s="2">
         <v>0.73499999999999999</v>
       </c>
-      <c r="C12" s="3">
-        <f>B11-B12</f>
+      <c r="C12" s="6">
+        <f t="shared" si="0"/>
         <v>2.6499999999999968E-2</v>
       </c>
     </row>
@@ -2114,8 +2116,8 @@
       <c r="B13" s="2">
         <v>0.70849996999999998</v>
       </c>
-      <c r="C13" s="3">
-        <f>B12-B13</f>
+      <c r="C13" s="6">
+        <f t="shared" si="0"/>
         <v>2.6500030000000008E-2</v>
       </c>
     </row>
@@ -2126,8 +2128,8 @@
       <c r="B14" s="2">
         <v>0.68200000000000005</v>
       </c>
-      <c r="C14" s="3">
-        <f>B13-B14</f>
+      <c r="C14" s="6">
+        <f t="shared" si="0"/>
         <v>2.6499969999999928E-2</v>
       </c>
     </row>
@@ -2138,8 +2140,8 @@
       <c r="B15" s="2">
         <v>0.65549999999999997</v>
       </c>
-      <c r="C15" s="3">
-        <f>B14-B15</f>
+      <c r="C15" s="6">
+        <f t="shared" si="0"/>
         <v>2.6500000000000079E-2</v>
       </c>
     </row>
@@ -2150,8 +2152,8 @@
       <c r="B16" s="2">
         <v>0.629</v>
       </c>
-      <c r="C16" s="3">
-        <f>B15-B16</f>
+      <c r="C16" s="6">
+        <f t="shared" si="0"/>
         <v>2.6499999999999968E-2</v>
       </c>
     </row>
@@ -2162,8 +2164,8 @@
       <c r="B17" s="2">
         <v>0.60249995999999995</v>
       </c>
-      <c r="C17" s="3">
-        <f>B16-B17</f>
+      <c r="C17" s="6">
+        <f t="shared" si="0"/>
         <v>2.6500040000000058E-2</v>
       </c>
     </row>
@@ -2174,8 +2176,8 @@
       <c r="B18" s="2">
         <v>0.57599999999999996</v>
       </c>
-      <c r="C18" s="3">
-        <f>B17-B18</f>
+      <c r="C18" s="6">
+        <f t="shared" si="0"/>
         <v>2.6499959999999989E-2</v>
       </c>
     </row>
@@ -2186,8 +2188,8 @@
       <c r="B19" s="2">
         <v>0.54949999999999999</v>
       </c>
-      <c r="C19" s="3">
-        <f>B18-B19</f>
+      <c r="C19" s="6">
+        <f t="shared" si="0"/>
         <v>2.6499999999999968E-2</v>
       </c>
     </row>
@@ -2198,8 +2200,8 @@
       <c r="B20" s="2">
         <v>0.52300000000000002</v>
       </c>
-      <c r="C20" s="3">
-        <f>B19-B20</f>
+      <c r="C20" s="6">
+        <f t="shared" si="0"/>
         <v>2.6499999999999968E-2</v>
       </c>
     </row>
@@ -2210,8 +2212,8 @@
       <c r="B21" s="2">
         <v>0.4965</v>
       </c>
-      <c r="C21" s="3">
-        <f>B20-B21</f>
+      <c r="C21" s="6">
+        <f t="shared" si="0"/>
         <v>2.6500000000000024E-2</v>
       </c>
     </row>
@@ -2222,8 +2224,8 @@
       <c r="B22" s="2">
         <v>0.47</v>
       </c>
-      <c r="C22" s="3">
-        <f>B21-B22</f>
+      <c r="C22" s="6">
+        <f t="shared" si="0"/>
         <v>2.6500000000000024E-2</v>
       </c>
     </row>
@@ -2234,8 +2236,8 @@
       <c r="B23" s="2">
         <v>0.45733332999999998</v>
       </c>
-      <c r="C23" s="3">
-        <f>B22-B23</f>
+      <c r="C23" s="6">
+        <f t="shared" si="0"/>
         <v>1.2666669999999991E-2</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -2249,8 +2251,8 @@
       <c r="B24" s="2">
         <v>0.44466665</v>
       </c>
-      <c r="C24" s="3">
-        <f>B23-B24</f>
+      <c r="C24" s="6">
+        <f t="shared" si="0"/>
         <v>1.2666679999999986E-2</v>
       </c>
     </row>
@@ -2261,8 +2263,8 @@
       <c r="B25" s="2">
         <v>0.43199998000000001</v>
       </c>
-      <c r="C25" s="3">
-        <f>B24-B25</f>
+      <c r="C25" s="6">
+        <f t="shared" si="0"/>
         <v>1.2666669999999991E-2</v>
       </c>
     </row>
@@ -2273,8 +2275,8 @@
       <c r="B26" s="2">
         <v>0.41933334</v>
       </c>
-      <c r="C26" s="3">
-        <f>B25-B26</f>
+      <c r="C26" s="6">
+        <f t="shared" si="0"/>
         <v>1.2666640000000007E-2</v>
       </c>
     </row>
@@ -2285,8 +2287,8 @@
       <c r="B27" s="2">
         <v>0.40666667000000001</v>
       </c>
-      <c r="C27" s="3">
-        <f>B26-B27</f>
+      <c r="C27" s="6">
+        <f t="shared" si="0"/>
         <v>1.2666669999999991E-2</v>
       </c>
     </row>
@@ -2297,8 +2299,8 @@
       <c r="B28" s="2">
         <v>0.39400000000000002</v>
       </c>
-      <c r="C28" s="3">
-        <f>B27-B28</f>
+      <c r="C28" s="6">
+        <f t="shared" si="0"/>
         <v>1.2666669999999991E-2</v>
       </c>
     </row>
@@ -2309,8 +2311,8 @@
       <c r="B29" s="2">
         <v>0.38133331999999998</v>
       </c>
-      <c r="C29" s="3">
-        <f>B28-B29</f>
+      <c r="C29" s="6">
+        <f t="shared" si="0"/>
         <v>1.2666680000000041E-2</v>
       </c>
     </row>
@@ -2321,8 +2323,8 @@
       <c r="B30" s="2">
         <v>0.36866668000000002</v>
       </c>
-      <c r="C30" s="3">
-        <f>B29-B30</f>
+      <c r="C30" s="6">
+        <f t="shared" si="0"/>
         <v>1.2666639999999951E-2</v>
       </c>
     </row>
@@ -2333,8 +2335,8 @@
       <c r="B31" s="2">
         <v>0.35599999999999998</v>
       </c>
-      <c r="C31" s="3">
-        <f>B30-B31</f>
+      <c r="C31" s="6">
+        <f t="shared" si="0"/>
         <v>1.2666680000000041E-2</v>
       </c>
     </row>
@@ -2345,8 +2347,8 @@
       <c r="B32" s="2">
         <v>0.34333332999999999</v>
       </c>
-      <c r="C32" s="3">
-        <f>B31-B32</f>
+      <c r="C32" s="6">
+        <f t="shared" si="0"/>
         <v>1.2666669999999991E-2</v>
       </c>
     </row>
@@ -2357,8 +2359,8 @@
       <c r="B33" s="2">
         <v>0.33066666</v>
       </c>
-      <c r="C33" s="3">
-        <f t="shared" ref="C33:C96" si="0">B32-B33</f>
+      <c r="C33" s="6">
+        <f t="shared" ref="C33:C96" si="1">B32-B33</f>
         <v>1.2666669999999991E-2</v>
       </c>
     </row>
@@ -2369,8 +2371,8 @@
       <c r="B34" s="2">
         <v>0.31800001999999999</v>
       </c>
-      <c r="C34" s="3">
-        <f t="shared" si="0"/>
+      <c r="C34" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666640000000007E-2</v>
       </c>
     </row>
@@ -2381,8 +2383,8 @@
       <c r="B35" s="2">
         <v>0.30533332000000002</v>
       </c>
-      <c r="C35" s="3">
-        <f t="shared" si="0"/>
+      <c r="C35" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666699999999975E-2</v>
       </c>
     </row>
@@ -2393,8 +2395,8 @@
       <c r="B36" s="2">
         <v>0.29266667000000002</v>
       </c>
-      <c r="C36" s="3">
-        <f t="shared" si="0"/>
+      <c r="C36" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666650000000002E-2</v>
       </c>
     </row>
@@ -2405,8 +2407,8 @@
       <c r="B37" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C37" s="3">
-        <f t="shared" si="0"/>
+      <c r="C37" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666669999999991E-2</v>
       </c>
     </row>
@@ -2417,8 +2419,8 @@
       <c r="B38" s="2">
         <v>0.26733332999999998</v>
       </c>
-      <c r="C38" s="3">
-        <f t="shared" si="0"/>
+      <c r="C38" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666670000000047E-2</v>
       </c>
     </row>
@@ -2429,8 +2431,8 @@
       <c r="B39" s="2">
         <v>0.25466670000000002</v>
       </c>
-      <c r="C39" s="3">
-        <f t="shared" si="0"/>
+      <c r="C39" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666629999999957E-2</v>
       </c>
     </row>
@@ -2441,8 +2443,8 @@
       <c r="B40" s="2">
         <v>0.24199999999999999</v>
       </c>
-      <c r="C40" s="3">
-        <f t="shared" si="0"/>
+      <c r="C40" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666700000000031E-2</v>
       </c>
     </row>
@@ -2453,8 +2455,8 @@
       <c r="B41" s="2">
         <v>0.22933334</v>
       </c>
-      <c r="C41" s="3">
-        <f t="shared" si="0"/>
+      <c r="C41" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666659999999996E-2</v>
       </c>
     </row>
@@ -2465,8 +2467,8 @@
       <c r="B42" s="2">
         <v>0.21666667000000001</v>
       </c>
-      <c r="C42" s="3">
-        <f t="shared" si="0"/>
+      <c r="C42" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666669999999991E-2</v>
       </c>
     </row>
@@ -2477,8 +2479,8 @@
       <c r="B43" s="2">
         <v>0.20399999999999999</v>
       </c>
-      <c r="C43" s="3">
-        <f t="shared" si="0"/>
+      <c r="C43" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666670000000019E-2</v>
       </c>
     </row>
@@ -2489,8 +2491,8 @@
       <c r="B44" s="2">
         <v>0.19133333999999999</v>
       </c>
-      <c r="C44" s="3">
-        <f t="shared" si="0"/>
+      <c r="C44" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666659999999996E-2</v>
       </c>
     </row>
@@ -2501,8 +2503,8 @@
       <c r="B45" s="2">
         <v>0.17866667</v>
       </c>
-      <c r="C45" s="3">
-        <f t="shared" si="0"/>
+      <c r="C45" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666669999999991E-2</v>
       </c>
     </row>
@@ -2513,8 +2515,8 @@
       <c r="B46" s="2">
         <v>0.16600003999999999</v>
       </c>
-      <c r="C46" s="3">
-        <f t="shared" si="0"/>
+      <c r="C46" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666630000000012E-2</v>
       </c>
     </row>
@@ -2525,8 +2527,8 @@
       <c r="B47" s="2">
         <v>0.15333334000000001</v>
       </c>
-      <c r="C47" s="3">
-        <f t="shared" si="0"/>
+      <c r="C47" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666699999999975E-2</v>
       </c>
     </row>
@@ -2537,8 +2539,8 @@
       <c r="B48" s="2">
         <v>0.14066661999999999</v>
       </c>
-      <c r="C48" s="3">
-        <f t="shared" si="0"/>
+      <c r="C48" s="6">
+        <f t="shared" si="1"/>
         <v>1.266672000000002E-2</v>
       </c>
     </row>
@@ -2549,8 +2551,8 @@
       <c r="B49" s="2">
         <v>0.128</v>
       </c>
-      <c r="C49" s="3">
-        <f t="shared" si="0"/>
+      <c r="C49" s="6">
+        <f t="shared" si="1"/>
         <v>1.266661999999999E-2</v>
       </c>
     </row>
@@ -2561,8 +2563,8 @@
       <c r="B50" s="2">
         <v>0.11533333</v>
       </c>
-      <c r="C50" s="3">
-        <f t="shared" si="0"/>
+      <c r="C50" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666670000000005E-2</v>
       </c>
     </row>
@@ -2573,8 +2575,8 @@
       <c r="B51" s="2">
         <v>0.102666624</v>
       </c>
-      <c r="C51" s="3">
-        <f t="shared" si="0"/>
+      <c r="C51" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666706E-2</v>
       </c>
     </row>
@@ -2585,8 +2587,8 @@
       <c r="B52" s="2">
         <v>0.09</v>
       </c>
-      <c r="C52" s="3">
-        <f t="shared" si="0"/>
+      <c r="C52" s="6">
+        <f t="shared" si="1"/>
         <v>1.2666624000000001E-2</v>
       </c>
     </row>
@@ -2597,8 +2599,8 @@
       <c r="B53" s="2">
         <v>8.5700004999999996E-2</v>
       </c>
-      <c r="C53" s="3">
-        <f t="shared" si="0"/>
+      <c r="C53" s="6">
+        <f t="shared" si="1"/>
         <v>4.2999950000000009E-3</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2612,8 +2614,8 @@
       <c r="B54" s="2">
         <v>8.1400020000000003E-2</v>
       </c>
-      <c r="C54" s="3">
-        <f t="shared" si="0"/>
+      <c r="C54" s="6">
+        <f t="shared" si="1"/>
         <v>4.2999849999999923E-3</v>
       </c>
     </row>
@@ -2624,8 +2626,8 @@
       <c r="B55" s="2">
         <v>7.7100009999999997E-2</v>
       </c>
-      <c r="C55" s="3">
-        <f t="shared" si="0"/>
+      <c r="C55" s="6">
+        <f t="shared" si="1"/>
         <v>4.3000100000000069E-3</v>
       </c>
     </row>
@@ -2636,8 +2638,8 @@
       <c r="B56" s="2">
         <v>7.2800000000000004E-2</v>
       </c>
-      <c r="C56" s="3">
-        <f t="shared" si="0"/>
+      <c r="C56" s="6">
+        <f t="shared" si="1"/>
         <v>4.300009999999993E-3</v>
       </c>
     </row>
@@ -2648,8 +2650,8 @@
       <c r="B57" s="2">
         <v>6.8500005000000003E-2</v>
       </c>
-      <c r="C57" s="3">
-        <f t="shared" si="0"/>
+      <c r="C57" s="6">
+        <f t="shared" si="1"/>
         <v>4.2999950000000009E-3</v>
       </c>
     </row>
@@ -2660,8 +2662,8 @@
       <c r="B58" s="2">
         <v>6.4199999999999993E-2</v>
       </c>
-      <c r="C58" s="3">
-        <f t="shared" si="0"/>
+      <c r="C58" s="6">
+        <f t="shared" si="1"/>
         <v>4.3000050000000095E-3</v>
       </c>
     </row>
@@ -2672,8 +2674,8 @@
       <c r="B59" s="2">
         <v>5.9900000000000002E-2</v>
       </c>
-      <c r="C59" s="3">
-        <f t="shared" si="0"/>
+      <c r="C59" s="6">
+        <f t="shared" si="1"/>
         <v>4.2999999999999913E-3</v>
       </c>
     </row>
@@ -2684,8 +2686,8 @@
       <c r="B60" s="2">
         <v>5.5600006E-2</v>
       </c>
-      <c r="C60" s="3">
-        <f t="shared" si="0"/>
+      <c r="C60" s="6">
+        <f t="shared" si="1"/>
         <v>4.2999940000000014E-3</v>
       </c>
     </row>
@@ -2696,8 +2698,8 @@
       <c r="B61" s="2">
         <v>5.1300004000000003E-2</v>
       </c>
-      <c r="C61" s="3">
-        <f t="shared" si="0"/>
+      <c r="C61" s="6">
+        <f t="shared" si="1"/>
         <v>4.3000019999999972E-3</v>
       </c>
     </row>
@@ -2708,8 +2710,8 @@
       <c r="B62" s="2">
         <v>4.7000001999999999E-2</v>
       </c>
-      <c r="C62" s="3">
-        <f t="shared" si="0"/>
+      <c r="C62" s="6">
+        <f t="shared" si="1"/>
         <v>4.3000020000000042E-3</v>
       </c>
     </row>
@@ -2720,8 +2722,8 @@
       <c r="B63" s="2">
         <v>4.2700000000000002E-2</v>
       </c>
-      <c r="C63" s="3">
-        <f t="shared" si="0"/>
+      <c r="C63" s="6">
+        <f t="shared" si="1"/>
         <v>4.3000019999999972E-3</v>
       </c>
     </row>
@@ -2732,8 +2734,8 @@
       <c r="B64" s="2">
         <v>3.8399999999999997E-2</v>
       </c>
-      <c r="C64" s="3">
-        <f t="shared" si="0"/>
+      <c r="C64" s="6">
+        <f t="shared" si="1"/>
         <v>4.3000000000000052E-3</v>
       </c>
     </row>
@@ -2744,8 +2746,8 @@
       <c r="B65" s="2">
         <v>3.4099999999999998E-2</v>
       </c>
-      <c r="C65" s="3">
-        <f t="shared" si="0"/>
+      <c r="C65" s="6">
+        <f t="shared" si="1"/>
         <v>4.2999999999999983E-3</v>
       </c>
     </row>
@@ -2756,8 +2758,8 @@
       <c r="B66" s="2">
         <v>2.9800002999999999E-2</v>
       </c>
-      <c r="C66" s="3">
-        <f t="shared" si="0"/>
+      <c r="C66" s="6">
+        <f t="shared" si="1"/>
         <v>4.2999969999999998E-3</v>
       </c>
     </row>
@@ -2768,8 +2770,8 @@
       <c r="B67" s="2">
         <v>2.5500001000000001E-2</v>
       </c>
-      <c r="C67" s="3">
-        <f t="shared" si="0"/>
+      <c r="C67" s="6">
+        <f t="shared" si="1"/>
         <v>4.3000019999999972E-3</v>
       </c>
     </row>
@@ -2780,8 +2782,8 @@
       <c r="B68" s="2">
         <v>2.1200001E-2</v>
       </c>
-      <c r="C68" s="3">
-        <f t="shared" si="0"/>
+      <c r="C68" s="6">
+        <f t="shared" si="1"/>
         <v>4.3000000000000017E-3</v>
       </c>
     </row>
@@ -2792,8 +2794,8 @@
       <c r="B69" s="2">
         <v>1.6900001000000001E-2</v>
       </c>
-      <c r="C69" s="3">
-        <f t="shared" si="0"/>
+      <c r="C69" s="6">
+        <f t="shared" si="1"/>
         <v>4.2999999999999983E-3</v>
       </c>
     </row>
@@ -2804,8 +2806,8 @@
       <c r="B70" s="2">
         <v>1.2600001E-2</v>
       </c>
-      <c r="C70" s="3">
-        <f t="shared" si="0"/>
+      <c r="C70" s="6">
+        <f t="shared" si="1"/>
         <v>4.3000000000000017E-3</v>
       </c>
     </row>
@@ -2816,8 +2818,8 @@
       <c r="B71" s="2">
         <v>8.3000009999999996E-3</v>
       </c>
-      <c r="C71" s="3">
-        <f t="shared" si="0"/>
+      <c r="C71" s="6">
+        <f t="shared" si="1"/>
         <v>4.3E-3</v>
       </c>
     </row>
@@ -2828,8 +2830,8 @@
       <c r="B72" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="C72" s="3">
-        <f t="shared" si="0"/>
+      <c r="C72" s="6">
+        <f t="shared" si="1"/>
         <v>4.3000009999999995E-3</v>
       </c>
     </row>
@@ -2840,8 +2842,8 @@
       <c r="B73" s="2">
         <v>3.888889E-3</v>
       </c>
-      <c r="C73" s="3">
-        <f t="shared" si="0"/>
+      <c r="C73" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111100000000011E-4</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2855,8 +2857,8 @@
       <c r="B74" s="2">
         <v>3.7777777999999998E-3</v>
       </c>
-      <c r="C74" s="3">
-        <f t="shared" si="0"/>
+      <c r="C74" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111120000000018E-4</v>
       </c>
     </row>
@@ -2867,8 +2869,8 @@
       <c r="B75" s="2">
         <v>3.6666670000000002E-3</v>
       </c>
-      <c r="C75" s="3">
-        <f t="shared" si="0"/>
+      <c r="C75" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111079999999961E-4</v>
       </c>
     </row>
@@ -2879,8 +2881,8 @@
       <c r="B76" s="2">
         <v>3.5555558E-3</v>
       </c>
-      <c r="C76" s="3">
-        <f t="shared" si="0"/>
+      <c r="C76" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111120000000018E-4</v>
       </c>
     </row>
@@ -2891,8 +2893,8 @@
       <c r="B77" s="2">
         <v>3.4444445999999998E-3</v>
       </c>
-      <c r="C77" s="3">
-        <f t="shared" si="0"/>
+      <c r="C77" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111120000000018E-4</v>
       </c>
     </row>
@@ -2903,8 +2905,8 @@
       <c r="B78" s="2">
         <v>3.3333334000000001E-3</v>
       </c>
-      <c r="C78" s="3">
-        <f t="shared" si="0"/>
+      <c r="C78" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111119999999974E-4</v>
       </c>
     </row>
@@ -2915,8 +2917,8 @@
       <c r="B79" s="2">
         <v>3.2222224E-3</v>
       </c>
-      <c r="C79" s="3">
-        <f t="shared" si="0"/>
+      <c r="C79" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111100000000011E-4</v>
       </c>
     </row>
@@ -2927,8 +2929,8 @@
       <c r="B80" s="2">
         <v>3.1111111999999998E-3</v>
       </c>
-      <c r="C80" s="3">
-        <f t="shared" si="0"/>
+      <c r="C80" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111120000000018E-4</v>
       </c>
     </row>
@@ -2939,8 +2941,8 @@
       <c r="B81" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="C81" s="3">
-        <f t="shared" si="0"/>
+      <c r="C81" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111119999999974E-4</v>
       </c>
     </row>
@@ -2951,8 +2953,8 @@
       <c r="B82" s="2">
         <v>2.888889E-3</v>
       </c>
-      <c r="C82" s="3">
-        <f t="shared" si="0"/>
+      <c r="C82" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111100000000011E-4</v>
       </c>
     </row>
@@ -2963,8 +2965,8 @@
       <c r="B83" s="2">
         <v>2.7777778000000002E-3</v>
       </c>
-      <c r="C83" s="3">
-        <f t="shared" si="0"/>
+      <c r="C83" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111119999999974E-4</v>
       </c>
     </row>
@@ -2975,8 +2977,8 @@
       <c r="B84" s="2">
         <v>2.6666669000000001E-3</v>
       </c>
-      <c r="C84" s="3">
-        <f t="shared" si="0"/>
+      <c r="C84" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111090000000007E-4</v>
       </c>
     </row>
@@ -2987,8 +2989,8 @@
       <c r="B85" s="2">
         <v>2.5555557E-3</v>
       </c>
-      <c r="C85" s="3">
-        <f t="shared" si="0"/>
+      <c r="C85" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111120000000018E-4</v>
       </c>
     </row>
@@ -2999,8 +3001,8 @@
       <c r="B86" s="2">
         <v>2.4444445000000002E-3</v>
       </c>
-      <c r="C86" s="3">
-        <f t="shared" si="0"/>
+      <c r="C86" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111119999999974E-4</v>
       </c>
     </row>
@@ -3011,8 +3013,8 @@
       <c r="B87" s="2">
         <v>2.3333333E-3</v>
       </c>
-      <c r="C87" s="3">
-        <f t="shared" si="0"/>
+      <c r="C87" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111120000000018E-4</v>
       </c>
     </row>
@@ -3023,8 +3025,8 @@
       <c r="B88" s="2">
         <v>2.2222225E-3</v>
       </c>
-      <c r="C88" s="3">
-        <f t="shared" si="0"/>
+      <c r="C88" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111080000000004E-4</v>
       </c>
     </row>
@@ -3035,8 +3037,8 @@
       <c r="B89" s="2">
         <v>2.1111112999999998E-3</v>
       </c>
-      <c r="C89" s="3">
-        <f t="shared" si="0"/>
+      <c r="C89" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111120000000018E-4</v>
       </c>
     </row>
@@ -3047,8 +3049,8 @@
       <c r="B90" s="2">
         <v>2E-3</v>
       </c>
-      <c r="C90" s="3">
-        <f t="shared" si="0"/>
+      <c r="C90" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111129999999978E-4</v>
       </c>
     </row>
@@ -3059,8 +3061,8 @@
       <c r="B91" s="2">
         <v>1.8888888999999999E-3</v>
       </c>
-      <c r="C91" s="3">
-        <f t="shared" si="0"/>
+      <c r="C91" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111110000000014E-4</v>
       </c>
     </row>
@@ -3071,8 +3073,8 @@
       <c r="B92" s="2">
         <v>1.7777779E-3</v>
       </c>
-      <c r="C92" s="3">
-        <f t="shared" si="0"/>
+      <c r="C92" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111099999999989E-4</v>
       </c>
     </row>
@@ -3083,8 +3085,8 @@
       <c r="B93" s="2">
         <v>1.6666667E-3</v>
       </c>
-      <c r="C93" s="3">
-        <f t="shared" si="0"/>
+      <c r="C93" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111119999999996E-4</v>
       </c>
     </row>
@@ -3095,8 +3097,8 @@
       <c r="B94" s="2">
         <v>1.5555555999999999E-3</v>
       </c>
-      <c r="C94" s="3">
-        <f t="shared" si="0"/>
+      <c r="C94" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111110000000014E-4</v>
       </c>
     </row>
@@ -3107,8 +3109,8 @@
       <c r="B95" s="2">
         <v>1.4444445E-3</v>
       </c>
-      <c r="C95" s="3">
-        <f t="shared" si="0"/>
+      <c r="C95" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111109999999993E-4</v>
       </c>
     </row>
@@ -3119,8 +3121,8 @@
       <c r="B96" s="2">
         <v>1.3333334000000001E-3</v>
       </c>
-      <c r="C96" s="3">
-        <f t="shared" si="0"/>
+      <c r="C96" s="6">
+        <f t="shared" si="1"/>
         <v>1.1111109999999993E-4</v>
       </c>
     </row>
@@ -3131,8 +3133,8 @@
       <c r="B97" s="2">
         <v>1.2222222000000001E-3</v>
       </c>
-      <c r="C97" s="3">
-        <f t="shared" ref="C97:C107" si="1">B96-B97</f>
+      <c r="C97" s="6">
+        <f t="shared" ref="C97:C100" si="2">B96-B97</f>
         <v>1.1111119999999996E-4</v>
       </c>
     </row>
@@ -3143,8 +3145,8 @@
       <c r="B98" s="2">
         <v>1.1111113E-3</v>
       </c>
-      <c r="C98" s="3">
-        <f t="shared" si="1"/>
+      <c r="C98" s="6">
+        <f t="shared" si="2"/>
         <v>1.1111090000000007E-4</v>
       </c>
     </row>
@@ -3155,8 +3157,8 @@
       <c r="B99" s="2">
         <v>1E-3</v>
       </c>
-      <c r="C99" s="3">
-        <f t="shared" si="1"/>
+      <c r="C99" s="6">
+        <f t="shared" si="2"/>
         <v>1.1111129999999999E-4</v>
       </c>
     </row>
@@ -3167,8 +3169,8 @@
       <c r="B100" s="2">
         <v>8.8888895999999996E-4</v>
       </c>
-      <c r="C100" s="3">
-        <f t="shared" si="1"/>
+      <c r="C100" s="6">
+        <f t="shared" si="2"/>
         <v>1.1111104000000006E-4</v>
       </c>
     </row>
@@ -3179,8 +3181,8 @@
       <c r="B101" s="2">
         <v>7.7777779999999995E-4</v>
       </c>
-      <c r="C101" s="3">
-        <f>B100-B101</f>
+      <c r="C101" s="6">
+        <f t="shared" ref="C101:C108" si="3">B100-B101</f>
         <v>1.1111116000000001E-4</v>
       </c>
     </row>
@@ -3191,8 +3193,8 @@
       <c r="B102" s="2">
         <v>6.6666670000000003E-4</v>
       </c>
-      <c r="C102" s="3">
-        <f>B101-B102</f>
+      <c r="C102" s="6">
+        <f t="shared" si="3"/>
         <v>1.1111109999999993E-4</v>
       </c>
     </row>
@@ -3203,8 +3205,8 @@
       <c r="B103" s="2">
         <v>5.5555559999999999E-4</v>
       </c>
-      <c r="C103" s="3">
-        <f>B102-B103</f>
+      <c r="C103" s="6">
+        <f t="shared" si="3"/>
         <v>1.1111110000000003E-4</v>
       </c>
     </row>
@@ -3215,8 +3217,8 @@
       <c r="B104" s="2">
         <v>4.4444447999999998E-4</v>
       </c>
-      <c r="C104" s="3">
-        <f>B103-B104</f>
+      <c r="C104" s="6">
+        <f t="shared" si="3"/>
         <v>1.1111112000000001E-4</v>
       </c>
     </row>
@@ -3227,8 +3229,8 @@
       <c r="B105" s="2">
         <v>3.3333336000000003E-4</v>
       </c>
-      <c r="C105" s="3">
-        <f>B104-B105</f>
+      <c r="C105" s="6">
+        <f t="shared" si="3"/>
         <v>1.1111111999999995E-4</v>
       </c>
     </row>
@@ -3239,8 +3241,8 @@
       <c r="B106" s="2">
         <v>2.2222223999999999E-4</v>
       </c>
-      <c r="C106" s="3">
-        <f>B105-B106</f>
+      <c r="C106" s="6">
+        <f t="shared" si="3"/>
         <v>1.1111112000000004E-4</v>
       </c>
     </row>
@@ -3251,8 +3253,8 @@
       <c r="B107" s="2">
         <v>1.1111112E-4</v>
       </c>
-      <c r="C107" s="3">
-        <f>B106-B107</f>
+      <c r="C107" s="6">
+        <f t="shared" si="3"/>
         <v>1.1111112E-4</v>
       </c>
     </row>
@@ -3263,8 +3265,8 @@
       <c r="B108" s="2">
         <v>0</v>
       </c>
-      <c r="C108" s="3">
-        <f>B107-B108</f>
+      <c r="C108" s="6">
+        <f t="shared" si="3"/>
         <v>1.1111112E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugfixes on encoder, changed from % to dB mapping.
</commit_message>
<xml_diff>
--- a/Documentation/DB_Mapping.xlsx
+++ b/Documentation/DB_Mapping.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oddbj\Documents\git\Revelator.io24.Api\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4957118-5490-469E-9FD6-BC6DE699BCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39AFB20-0285-4504-BD50-A48C9CBD71C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-9810" windowWidth="21840" windowHeight="38040" xr2:uid="{4EF7F543-1A19-4AA0-AC06-25240FBC5CDA}"/>
+    <workbookView xWindow="-19560" yWindow="435" windowWidth="20535" windowHeight="14850" activeTab="1" xr2:uid="{4EF7F543-1A19-4AA0-AC06-25240FBC5CDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Volume Mic L" sheetId="1" r:id="rId1"/>
+    <sheet name="Volume Main Out" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>dB</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>Change in scale</t>
+  </si>
+  <si>
+    <t>Change in scale?</t>
+  </si>
+  <si>
+    <t>Something changes around here.</t>
   </si>
 </sst>
 </file>
@@ -210,13 +216,23 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nb-NO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.6088720686679536E-2"/>
+          <c:y val="7.2051830407129855E-2"/>
+          <c:w val="0.91936449857207481"/>
+          <c:h val="0.87957136937796832"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -960,7 +976,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nb-NO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1062180511"/>
@@ -1018,7 +1034,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nb-NO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1062177599"/>
@@ -1070,7 +1086,908 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nb-NO"/>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Volume Main Out'!$A$2:$A$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="97"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Volume Main Out'!$B$2:$B$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="97"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.86863946999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78523209999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.72398359999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67555699999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.63550435999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60135039999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57157919999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.54519280000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.52149944999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.48032236</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.46218184000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.44535550000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.42966574000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.41496870000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.40114620000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.3881</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.37574746999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.36401860000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.35285339999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.34220020000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.33201402000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.32225569999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.31289076999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.30388864999999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.29522228</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.2868676</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.27880290000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.27100869999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.26346752000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.25616336000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.24908184999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.24220976</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.23553511999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.22904682000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.22273481000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.21658973000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.21060297</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.20476659999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.19907322999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.19351603000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.18808863000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.18278512</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.17759997</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.17252793999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.16756433000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.16270451</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.15794425000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.15327953999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.14870667000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.14422204</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.13982228999999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.13550435999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.13126518000000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.12710193</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.123011984</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.1189928</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.11504193</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.11115710400000001</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.10733616999999999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.10357706999999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9.9877789999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>9.6236489999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>9.2651369999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>8.9120740000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>8.5642930000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8.2216404000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>7.8839699999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>7.5511343999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7.2229979999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>6.8994319999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6.5803109999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6.265511E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.9549199999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5.6484251999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.3459223E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5.0473052999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4.7524772999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.4613432000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.1738126E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.8897958000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.6092079999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.3319682000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.0579986E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.7872203000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2.519561E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.2549512000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.993319E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.7346001999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.4787302E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.22564845E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.75292E-3</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>7.2760424000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4.8252883999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2.4001259999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B736-4D17-A5EC-4783B67BFE3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="814499471"/>
+        <c:axId val="997938095"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="814499471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="997938095"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="997938095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="814499471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1121,7 +2038,543 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1658,6 +3111,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB1673E5-7945-F40A-0908-AB4F96E0E353}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1957,8 +3451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91BCD35-61D8-49E2-AC48-51ABA70835B2}">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3275,4 +4769,1231 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05FCF0E-0E6C-410F-9544-A88F233C49D0}">
+  <dimension ref="A1:F98"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.86863946999999997</v>
+      </c>
+      <c r="C3" s="6">
+        <f t="shared" ref="C3:F66" si="0">B2-B3</f>
+        <v>0.13136053000000003</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.78523209999999999</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" si="0"/>
+        <v>8.3407369999999981E-2</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.72398359999999995</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="0"/>
+        <v>6.1248500000000039E-2</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.67555699999999996</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="0"/>
+        <v>4.8426599999999986E-2</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.63550435999999999</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="0"/>
+        <v>4.0052639999999973E-2</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.60135039999999995</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" si="0"/>
+        <v>3.4153960000000039E-2</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.57157919999999995</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="0"/>
+        <v>2.9771199999999998E-2</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.54519280000000003</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" si="0"/>
+        <v>2.6386399999999921E-2</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.52149944999999998</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="0"/>
+        <v>2.3693350000000057E-2</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" si="0"/>
+        <v>2.1499449999999976E-2</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.48032236</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9677639999999996E-2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.46218184000000001</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="0"/>
+        <v>1.8140519999999993E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.44535550000000002</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6826339999999995E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.42966574000000002</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" si="0"/>
+        <v>1.5689759999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.41496870000000002</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="0"/>
+        <v>1.4697039999999995E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.40114620000000001</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3822500000000015E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.3881</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3046200000000008E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.37574746999999997</v>
+      </c>
+      <c r="C20" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2352530000000028E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>-19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.36401860000000003</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1728869999999947E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>-20</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.35285339999999998</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1165200000000042E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>-21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.34220020000000001</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0653199999999974E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>-22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.33201402000000002</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0186179999999989E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>-23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.32225569999999998</v>
+      </c>
+      <c r="C25" s="6">
+        <f t="shared" si="0"/>
+        <v>9.7583200000000425E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>-24</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.31289076999999998</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" si="0"/>
+        <v>9.3649299999999935E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>-25</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.30388864999999998</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="0"/>
+        <v>9.0021200000000023E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>-26</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.29522228</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="0"/>
+        <v>8.6663699999999788E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>-27</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.2868676</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="0"/>
+        <v>8.3546800000000032E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>-28</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.27880290000000002</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="0"/>
+        <v>8.0646999999999802E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>-29</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.27100869999999999</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="0"/>
+        <v>7.7942000000000289E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>-30</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.26346752000000001</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="0"/>
+        <v>7.5411799999999807E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>-31</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.25616336000000001</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="0"/>
+        <v>7.304160000000004E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>-32</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.24908184999999999</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="0"/>
+        <v>7.0815100000000131E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>-33</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.24220976</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" si="0"/>
+        <v>6.8720899999999974E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>-34</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.23553511999999999</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" si="0"/>
+        <v>6.6746400000000095E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>-35</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.22904682000000001</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" si="0"/>
+        <v>6.4882999999999746E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>-36</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.22273481000000001</v>
+      </c>
+      <c r="C38" s="6">
+        <f t="shared" si="0"/>
+        <v>6.3120100000000068E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>-37</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.21658973000000001</v>
+      </c>
+      <c r="C39" s="6">
+        <f t="shared" si="0"/>
+        <v>6.1450799999999972E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>-38</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.21060297</v>
+      </c>
+      <c r="C40" s="6">
+        <f t="shared" si="0"/>
+        <v>5.9867600000000076E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>-39</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.20476659999999999</v>
+      </c>
+      <c r="C41" s="6">
+        <f t="shared" si="0"/>
+        <v>5.8363700000000074E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>-40</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.19907322999999999</v>
+      </c>
+      <c r="C42" s="6">
+        <f t="shared" si="0"/>
+        <v>5.6933700000000032E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>-41</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.19351603000000001</v>
+      </c>
+      <c r="C43" s="6">
+        <f t="shared" si="0"/>
+        <v>5.5571999999999844E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>-42</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.18808863000000001</v>
+      </c>
+      <c r="C44" s="6">
+        <f t="shared" si="0"/>
+        <v>5.4273999999999989E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>-43</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.18278512</v>
+      </c>
+      <c r="C45" s="6">
+        <f t="shared" si="0"/>
+        <v>5.3035100000000113E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>-44</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.17759997</v>
+      </c>
+      <c r="C46" s="6">
+        <f t="shared" si="0"/>
+        <v>5.1851499999999995E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>-45</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.17252793999999999</v>
+      </c>
+      <c r="C47" s="6">
+        <f t="shared" si="0"/>
+        <v>5.0720300000000051E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>-46</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.16756433000000001</v>
+      </c>
+      <c r="C48" s="6">
+        <f t="shared" si="0"/>
+        <v>4.9636099999999794E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>-47</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.16270451</v>
+      </c>
+      <c r="C49" s="6">
+        <f t="shared" si="0"/>
+        <v>4.8598200000000147E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>-48</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.15794425000000001</v>
+      </c>
+      <c r="C50" s="6">
+        <f t="shared" si="0"/>
+        <v>4.7602599999999884E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>-49</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.15327953999999999</v>
+      </c>
+      <c r="C51" s="6">
+        <f t="shared" si="0"/>
+        <v>4.6647100000000163E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>-50</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.14870667000000001</v>
+      </c>
+      <c r="C52" s="6">
+        <f t="shared" si="0"/>
+        <v>4.5728699999999789E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>-51</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.14422204</v>
+      </c>
+      <c r="C53" s="6">
+        <f t="shared" si="0"/>
+        <v>4.4846300000000172E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>-52</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.13982228999999999</v>
+      </c>
+      <c r="C54" s="6">
+        <f t="shared" si="0"/>
+        <v>4.3997500000000078E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>-53</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.13550435999999999</v>
+      </c>
+      <c r="C55" s="6">
+        <f t="shared" si="0"/>
+        <v>4.3179299999999976E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>-54</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.13126518000000001</v>
+      </c>
+      <c r="C56" s="6">
+        <f t="shared" si="0"/>
+        <v>4.2391799999999813E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>-55</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0.12710193</v>
+      </c>
+      <c r="C57" s="6">
+        <f t="shared" si="0"/>
+        <v>4.1632500000000072E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>-56</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0.123011984</v>
+      </c>
+      <c r="C58" s="6">
+        <f t="shared" si="0"/>
+        <v>4.0899459999999971E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>-57</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0.1189928</v>
+      </c>
+      <c r="C59" s="6">
+        <f t="shared" si="0"/>
+        <v>4.019184000000009E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>-58</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0.11504193</v>
+      </c>
+      <c r="C60" s="6">
+        <f t="shared" si="0"/>
+        <v>3.9508699999999952E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>-59</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0.11115710400000001</v>
+      </c>
+      <c r="C61" s="6">
+        <f t="shared" si="0"/>
+        <v>3.884825999999994E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>-60</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0.10733616999999999</v>
+      </c>
+      <c r="C62" s="6">
+        <f t="shared" si="0"/>
+        <v>3.8209340000000119E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>-61</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0.10357706999999999</v>
+      </c>
+      <c r="C63" s="6">
+        <f t="shared" si="0"/>
+        <v>3.7591000000000013E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>-62</v>
+      </c>
+      <c r="B64" s="1">
+        <v>9.9877789999999994E-2</v>
+      </c>
+      <c r="C64" s="6">
+        <f t="shared" si="0"/>
+        <v>3.6992799999999992E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>-63</v>
+      </c>
+      <c r="B65" s="1">
+        <v>9.6236489999999994E-2</v>
+      </c>
+      <c r="C65" s="6">
+        <f t="shared" si="0"/>
+        <v>3.6413000000000001E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>-64</v>
+      </c>
+      <c r="B66" s="1">
+        <v>9.2651369999999997E-2</v>
+      </c>
+      <c r="C66" s="6">
+        <f t="shared" si="0"/>
+        <v>3.5851199999999972E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>-65</v>
+      </c>
+      <c r="B67" s="1">
+        <v>8.9120740000000004E-2</v>
+      </c>
+      <c r="C67" s="6">
+        <f t="shared" ref="C67:C98" si="1">B66-B67</f>
+        <v>3.5306299999999929E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>-66</v>
+      </c>
+      <c r="B68" s="1">
+        <v>8.5642930000000006E-2</v>
+      </c>
+      <c r="C68" s="6">
+        <f t="shared" si="1"/>
+        <v>3.4778099999999978E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>-67</v>
+      </c>
+      <c r="B69" s="1">
+        <v>8.2216404000000007E-2</v>
+      </c>
+      <c r="C69" s="6">
+        <f t="shared" si="1"/>
+        <v>3.4265259999999992E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>-68</v>
+      </c>
+      <c r="B70" s="1">
+        <v>7.8839699999999999E-2</v>
+      </c>
+      <c r="C70" s="6">
+        <f t="shared" si="1"/>
+        <v>3.3767040000000081E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>-69</v>
+      </c>
+      <c r="B71" s="1">
+        <v>7.5511343999999994E-2</v>
+      </c>
+      <c r="C71" s="6">
+        <f t="shared" si="1"/>
+        <v>3.3283560000000045E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>-70</v>
+      </c>
+      <c r="B72" s="1">
+        <v>7.2229979999999999E-2</v>
+      </c>
+      <c r="C72" s="6">
+        <f t="shared" si="1"/>
+        <v>3.281363999999995E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>-71</v>
+      </c>
+      <c r="B73" s="1">
+        <v>6.8994319999999998E-2</v>
+      </c>
+      <c r="C73" s="6">
+        <f t="shared" si="1"/>
+        <v>3.2356600000000013E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>-72</v>
+      </c>
+      <c r="B74" s="1">
+        <v>6.5803109999999998E-2</v>
+      </c>
+      <c r="C74" s="6">
+        <f t="shared" si="1"/>
+        <v>3.1912099999999999E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>-73</v>
+      </c>
+      <c r="B75" s="1">
+        <v>6.265511E-2</v>
+      </c>
+      <c r="C75" s="6">
+        <f t="shared" si="1"/>
+        <v>3.147999999999998E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>-74</v>
+      </c>
+      <c r="B76" s="1">
+        <v>5.9549199999999997E-2</v>
+      </c>
+      <c r="C76" s="6">
+        <f t="shared" si="1"/>
+        <v>3.1059100000000034E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>-75</v>
+      </c>
+      <c r="B77" s="1">
+        <v>5.6484251999999999E-2</v>
+      </c>
+      <c r="C77" s="6">
+        <f t="shared" si="1"/>
+        <v>3.0649479999999979E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>-76</v>
+      </c>
+      <c r="B78" s="1">
+        <v>5.3459223E-2</v>
+      </c>
+      <c r="C78" s="6">
+        <f t="shared" si="1"/>
+        <v>3.0250289999999985E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>-77</v>
+      </c>
+      <c r="B79" s="1">
+        <v>5.0473052999999997E-2</v>
+      </c>
+      <c r="C79" s="6">
+        <f t="shared" si="1"/>
+        <v>2.9861700000000033E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>-78</v>
+      </c>
+      <c r="B80" s="1">
+        <v>4.7524772999999999E-2</v>
+      </c>
+      <c r="C80" s="6">
+        <f t="shared" si="1"/>
+        <v>2.9482799999999976E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>-79</v>
+      </c>
+      <c r="B81" s="1">
+        <v>4.4613432000000001E-2</v>
+      </c>
+      <c r="C81" s="6">
+        <f t="shared" si="1"/>
+        <v>2.9113409999999978E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>-80</v>
+      </c>
+      <c r="B82" s="1">
+        <v>4.1738126E-2</v>
+      </c>
+      <c r="C82" s="6">
+        <f t="shared" si="1"/>
+        <v>2.8753060000000011E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>-81</v>
+      </c>
+      <c r="B83" s="1">
+        <v>3.8897958000000003E-2</v>
+      </c>
+      <c r="C83" s="6">
+        <f t="shared" si="1"/>
+        <v>2.8401679999999971E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>-82</v>
+      </c>
+      <c r="B84" s="1">
+        <v>3.6092079999999999E-2</v>
+      </c>
+      <c r="C84" s="6">
+        <f t="shared" si="1"/>
+        <v>2.8058780000000047E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>-83</v>
+      </c>
+      <c r="B85" s="1">
+        <v>3.3319682000000003E-2</v>
+      </c>
+      <c r="C85" s="6">
+        <f t="shared" si="1"/>
+        <v>2.7723979999999954E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>-84</v>
+      </c>
+      <c r="B86" s="1">
+        <v>3.0579986E-2</v>
+      </c>
+      <c r="C86" s="6">
+        <f t="shared" si="1"/>
+        <v>2.7396960000000033E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>-85</v>
+      </c>
+      <c r="B87" s="1">
+        <v>2.7872203000000002E-2</v>
+      </c>
+      <c r="C87" s="6">
+        <f t="shared" si="1"/>
+        <v>2.7077829999999983E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>-86</v>
+      </c>
+      <c r="B88" s="1">
+        <v>2.519561E-2</v>
+      </c>
+      <c r="C88" s="6">
+        <f t="shared" si="1"/>
+        <v>2.6765930000000014E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>-87</v>
+      </c>
+      <c r="B89" s="1">
+        <v>2.2549512000000001E-2</v>
+      </c>
+      <c r="C89" s="6">
+        <f t="shared" si="1"/>
+        <v>2.6460979999999995E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>-88</v>
+      </c>
+      <c r="B90" s="1">
+        <v>1.993319E-2</v>
+      </c>
+      <c r="C90" s="6">
+        <f t="shared" si="1"/>
+        <v>2.6163220000000008E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>-89</v>
+      </c>
+      <c r="B91" s="1">
+        <v>1.7346001999999999E-2</v>
+      </c>
+      <c r="C91" s="6">
+        <f t="shared" si="1"/>
+        <v>2.5871880000000007E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>-90</v>
+      </c>
+      <c r="B92" s="1">
+        <v>1.4787302E-2</v>
+      </c>
+      <c r="C92" s="6">
+        <f t="shared" si="1"/>
+        <v>2.5586999999999988E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>-91</v>
+      </c>
+      <c r="B93" s="1">
+        <v>1.22564845E-2</v>
+      </c>
+      <c r="C93" s="6">
+        <f t="shared" si="1"/>
+        <v>2.5308175000000009E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>-92</v>
+      </c>
+      <c r="B94" s="1">
+        <v>9.75292E-3</v>
+      </c>
+      <c r="C94" s="6">
+        <f t="shared" si="1"/>
+        <v>2.5035644999999995E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>-93</v>
+      </c>
+      <c r="B95" s="1">
+        <v>7.2760424000000001E-3</v>
+      </c>
+      <c r="C95" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4768775999999999E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>-94</v>
+      </c>
+      <c r="B96" s="1">
+        <v>4.8252883999999998E-3</v>
+      </c>
+      <c r="C96" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4507540000000003E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>-95</v>
+      </c>
+      <c r="B97" s="1">
+        <v>2.4001259999999998E-3</v>
+      </c>
+      <c r="C97" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4251623999999999E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>-96</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0</v>
+      </c>
+      <c r="C98" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4001259999999998E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>